<commit_message>
Scaling so STM doesn't have to deal with negative numbers - rev equation and functins
</commit_message>
<xml_diff>
--- a/Projects/Proj6/voltageVSccr.xlsx
+++ b/Projects/Proj6/voltageVSccr.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>Rounded</t>
   </si>
@@ -37,15 +37,37 @@
   <si>
     <t>y=-1.7x+12.727</t>
   </si>
+  <si>
+    <t>Exact CCR</t>
+  </si>
+  <si>
+    <t>Scaled +5 *2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -68,13 +90,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -271,11 +297,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1211925840"/>
-        <c:axId val="-1211928320"/>
+        <c:axId val="1739426144"/>
+        <c:axId val="1739095568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1211925840"/>
+        <c:axId val="1739426144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -331,12 +357,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1211928320"/>
+        <c:crossAx val="1739095568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1211928320"/>
+        <c:axId val="1739095568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -392,7 +418,392 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1211925840"/>
+        <c:crossAx val="1739426144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$17:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$17:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1779231952"/>
+        <c:axId val="1779228912"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1779231952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1779228912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1779228912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1779231952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -481,7 +892,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1024,6 +1991,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1295,10 +2292,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1343,7 +2340,7 @@
         <v>19.8</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D12" si="1">ROUND(C2,0)</f>
+        <f t="shared" ref="D2:D11" si="1">ROUND(C2,0)</f>
         <v>20</v>
       </c>
       <c r="E2">
@@ -1372,7 +2369,7 @@
         <v>18</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E2:E12" si="4">(-1.7*A3)+12.727</f>
+        <f t="shared" ref="E3:E11" si="4">(-1.7*A3)+12.727</f>
         <v>17.826999999999998</v>
       </c>
       <c r="F3">
@@ -1591,6 +2588,257 @@
       </c>
       <c r="F12" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <f>(A1+5)*2</f>
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>21</v>
+      </c>
+      <c r="C17">
+        <f>ROUND(B17,0)</f>
+        <v>21</v>
+      </c>
+      <c r="E17">
+        <f>-0.8409*A17+21.136</f>
+        <v>21.135999999999999</v>
+      </c>
+      <c r="F17">
+        <f>ROUND(E17,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <f t="shared" ref="A18:A27" si="6">(A2+5)*2</f>
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <f>B17-(8/5)</f>
+        <v>19.399999999999999</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:C27" si="7">ROUND(B18,0)</f>
+        <v>19</v>
+      </c>
+      <c r="E18">
+        <f>-0.8409*A18+21.136</f>
+        <v>19.4542</v>
+      </c>
+      <c r="F18">
+        <f t="shared" ref="F18:F27" si="8">ROUND(E18,0)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <f t="shared" ref="B19:B21" si="9">B18-(8/5)</f>
+        <v>17.799999999999997</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="7"/>
+        <v>18</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ref="E19:E27" si="10">-0.8409*A19+21.136</f>
+        <v>17.772399999999998</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="8"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="9"/>
+        <v>16.199999999999996</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="10"/>
+        <v>16.090599999999998</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="9"/>
+        <v>14.599999999999996</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="10"/>
+        <v>14.408799999999999</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="B22">
+        <v>13</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="7"/>
+        <v>13</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="10"/>
+        <v>12.727</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="B23">
+        <f>B22-(9/5)</f>
+        <v>11.2</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="10"/>
+        <v>11.045199999999999</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+      <c r="B24">
+        <f t="shared" ref="B24:B27" si="11">B23-(9/5)</f>
+        <v>9.3999999999999986</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="10"/>
+        <v>9.3633999999999986</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="11"/>
+        <v>7.5999999999999988</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="10"/>
+        <v>7.6815999999999995</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="11"/>
+        <v>5.7999999999999989</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="10"/>
+        <v>5.9998000000000005</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="11"/>
+        <v>3.9999999999999991</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="10"/>
+        <v>4.3180000000000014</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="8"/>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Scaling now to 8 bits
</commit_message>
<xml_diff>
--- a/Projects/Proj6/voltageVSccr.xlsx
+++ b/Projects/Proj6/voltageVSccr.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>Rounded</t>
   </si>
@@ -48,7 +48,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -72,6 +72,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -90,17 +97,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -297,11 +309,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1739426144"/>
-        <c:axId val="1739095568"/>
+        <c:axId val="-806179856"/>
+        <c:axId val="-806177536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1739426144"/>
+        <c:axId val="-806179856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -357,12 +369,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1739095568"/>
+        <c:crossAx val="-806177536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1739095568"/>
+        <c:axId val="-806177536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -382,6 +394,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -418,7 +431,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1739426144"/>
+        <c:crossAx val="-806179856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -590,7 +603,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$17:$A$27</c:f>
+              <c:f>Sheet1!$A$30:$A$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -598,41 +611,41 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>26.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0</c:v>
+                  <c:v>77.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.0</c:v>
+                  <c:v>102.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.0</c:v>
+                  <c:v>128.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.0</c:v>
+                  <c:v>153.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.0</c:v>
+                  <c:v>179.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16.0</c:v>
+                  <c:v>204.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18.0</c:v>
+                  <c:v>230.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20.0</c:v>
+                  <c:v>255.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$27</c:f>
+              <c:f>Sheet1!$B$30:$B$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -640,34 +653,34 @@
                   <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.0</c:v>
+                  <c:v>19.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.0</c:v>
+                  <c:v>17.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.0</c:v>
+                  <c:v>16.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15.0</c:v>
+                  <c:v>14.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.0</c:v>
+                  <c:v>11.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.0</c:v>
+                  <c:v>9.399999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.0</c:v>
+                  <c:v>7.599999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.0</c:v>
+                  <c:v>5.799999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.0</c:v>
+                  <c:v>3.999999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -682,11 +695,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1779231952"/>
-        <c:axId val="1779228912"/>
+        <c:axId val="-805356544"/>
+        <c:axId val="-784304576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1779231952"/>
+        <c:axId val="-805356544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -742,12 +755,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1779228912"/>
+        <c:crossAx val="-784304576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1779228912"/>
+        <c:axId val="-784304576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -803,7 +816,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1779231952"/>
+        <c:crossAx val="-805356544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1998,20 +2011,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2292,10 +2305,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30:D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2600,141 +2613,114 @@
       <c r="C16" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D16" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
-        <f>(A1+5)*2</f>
+        <f>(A1+5)*25.5</f>
         <v>0</v>
       </c>
       <c r="B17">
         <v>21</v>
       </c>
       <c r="C17">
-        <f>ROUND(B17,0)</f>
+        <f>ROUND(A17,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
         <v>21</v>
       </c>
-      <c r="E17">
-        <f>-0.8409*A17+21.136</f>
-        <v>21.135999999999999</v>
-      </c>
-      <c r="F17">
-        <f>ROUND(E17,0)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
-        <f t="shared" ref="A18:A27" si="6">(A2+5)*2</f>
-        <v>2</v>
+        <f t="shared" ref="A18:A27" si="6">(A2+5)*25.5</f>
+        <v>25.5</v>
       </c>
       <c r="B18">
         <f>B17-(8/5)</f>
         <v>19.399999999999999</v>
       </c>
       <c r="C18">
-        <f t="shared" ref="C18:C27" si="7">ROUND(B18,0)</f>
+        <f t="shared" ref="C18:C27" si="7">ROUND(A18,0)</f>
+        <v>26</v>
+      </c>
+      <c r="D18" s="1">
         <v>19</v>
       </c>
-      <c r="E18">
-        <f>-0.8409*A18+21.136</f>
-        <v>19.4542</v>
-      </c>
-      <c r="F18">
-        <f t="shared" ref="F18:F27" si="8">ROUND(E18,0)</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="B19">
-        <f t="shared" ref="B19:B21" si="9">B18-(8/5)</f>
+        <f t="shared" ref="B19:B21" si="8">B18-(8/5)</f>
         <v>17.799999999999997</v>
       </c>
       <c r="C19">
         <f t="shared" si="7"/>
+        <v>51</v>
+      </c>
+      <c r="D19" s="1">
         <v>18</v>
       </c>
-      <c r="E19">
-        <f t="shared" ref="E19:E27" si="10">-0.8409*A19+21.136</f>
-        <v>17.772399999999998</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="8"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>76.5</v>
       </c>
       <c r="B20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>16.199999999999996</v>
       </c>
       <c r="C20">
         <f t="shared" si="7"/>
+        <v>77</v>
+      </c>
+      <c r="D20" s="1">
         <v>16</v>
       </c>
-      <c r="E20">
-        <f t="shared" si="10"/>
-        <v>16.090599999999998</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="8"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v>102</v>
       </c>
       <c r="B21">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>14.599999999999996</v>
       </c>
       <c r="C21">
         <f t="shared" si="7"/>
+        <v>102</v>
+      </c>
+      <c r="D21" s="1">
         <v>15</v>
       </c>
-      <c r="E21">
-        <f t="shared" si="10"/>
-        <v>14.408799999999999</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="8"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="6"/>
-        <v>10</v>
+        <v>127.5</v>
       </c>
       <c r="B22">
         <v>13</v>
       </c>
       <c r="C22">
         <f t="shared" si="7"/>
+        <v>128</v>
+      </c>
+      <c r="D22" s="1">
         <v>13</v>
       </c>
-      <c r="E22">
-        <f t="shared" si="10"/>
-        <v>12.727</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="8"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="6"/>
-        <v>12</v>
+        <v>153</v>
       </c>
       <c r="B23">
         <f>B22-(9/5)</f>
@@ -2742,102 +2728,281 @@
       </c>
       <c r="C23">
         <f t="shared" si="7"/>
+        <v>153</v>
+      </c>
+      <c r="D23" s="1">
         <v>11</v>
       </c>
-      <c r="E23">
-        <f t="shared" si="10"/>
-        <v>11.045199999999999</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="8"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="6"/>
-        <v>14</v>
+        <v>178.5</v>
       </c>
       <c r="B24">
-        <f t="shared" ref="B24:B27" si="11">B23-(9/5)</f>
+        <f t="shared" ref="B24:B27" si="9">B23-(9/5)</f>
         <v>9.3999999999999986</v>
       </c>
       <c r="C24">
         <f t="shared" si="7"/>
+        <v>179</v>
+      </c>
+      <c r="D24" s="1">
         <v>9</v>
       </c>
-      <c r="E24">
-        <f t="shared" si="10"/>
-        <v>9.3633999999999986</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="8"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="6"/>
-        <v>16</v>
+        <v>204</v>
       </c>
       <c r="B25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>7.5999999999999988</v>
       </c>
       <c r="C25">
         <f t="shared" si="7"/>
+        <v>204</v>
+      </c>
+      <c r="D25" s="1">
         <v>8</v>
       </c>
-      <c r="E25">
-        <f t="shared" si="10"/>
-        <v>7.6815999999999995</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="8"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="6"/>
-        <v>18</v>
+        <v>229.5</v>
       </c>
       <c r="B26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>5.7999999999999989</v>
       </c>
       <c r="C26">
         <f t="shared" si="7"/>
+        <v>230</v>
+      </c>
+      <c r="D26" s="1">
         <v>6</v>
       </c>
-      <c r="E26">
-        <f t="shared" si="10"/>
-        <v>5.9998000000000005</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="8"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="6"/>
-        <v>20</v>
+        <v>255</v>
       </c>
       <c r="B27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>3.9999999999999991</v>
       </c>
       <c r="C27">
         <f t="shared" si="7"/>
+        <v>255</v>
+      </c>
+      <c r="D27" s="1">
         <v>4</v>
       </c>
-      <c r="E27">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <f>ROUND(A17,0)</f>
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>21</v>
+      </c>
+      <c r="D30">
+        <f>-0.0667*A30+21.242</f>
+        <v>21.242000000000001</v>
+      </c>
+      <c r="E30">
+        <f>ROUND(D30,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <f t="shared" ref="A31:A40" si="10">ROUND(A18,0)</f>
+        <v>26</v>
+      </c>
+      <c r="B31">
+        <f>B30-(8/5)</f>
+        <v>19.399999999999999</v>
+      </c>
+      <c r="D31">
+        <f t="shared" ref="D31:D40" si="11">-0.0667*A31+21.242</f>
+        <v>19.5078</v>
+      </c>
+      <c r="E31">
+        <f t="shared" ref="E31:E40" si="12">ROUND(D31,0)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32">
         <f t="shared" si="10"/>
-        <v>4.3180000000000014</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="8"/>
+        <v>51</v>
+      </c>
+      <c r="B32">
+        <f t="shared" ref="B32:B34" si="13">B31-(8/5)</f>
+        <v>17.799999999999997</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="11"/>
+        <v>17.840299999999999</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="12"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <f t="shared" si="10"/>
+        <v>77</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="13"/>
+        <v>16.199999999999996</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="11"/>
+        <v>16.106100000000001</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="12"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <f t="shared" si="10"/>
+        <v>102</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="13"/>
+        <v>14.599999999999996</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="11"/>
+        <v>14.438600000000001</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="12"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <f t="shared" si="10"/>
+        <v>128</v>
+      </c>
+      <c r="B35">
+        <v>13</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="11"/>
+        <v>12.704400000000001</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="12"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <f t="shared" si="10"/>
+        <v>153</v>
+      </c>
+      <c r="B36">
+        <f>B35-(9/5)</f>
+        <v>11.2</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="11"/>
+        <v>11.036900000000001</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="12"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <f t="shared" si="10"/>
+        <v>179</v>
+      </c>
+      <c r="B37">
+        <f t="shared" ref="B37:B40" si="14">B36-(9/5)</f>
+        <v>9.3999999999999986</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="11"/>
+        <v>9.3027000000000015</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="12"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <f t="shared" si="10"/>
+        <v>204</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="14"/>
+        <v>7.5999999999999988</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="11"/>
+        <v>7.6352000000000011</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="12"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <f t="shared" si="10"/>
+        <v>230</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="14"/>
+        <v>5.7999999999999989</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="11"/>
+        <v>5.9010000000000016</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <f t="shared" si="10"/>
+        <v>255</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="14"/>
+        <v>3.9999999999999991</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="11"/>
+        <v>4.2335000000000029</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Redid QNX portion for validity
</commit_message>
<xml_diff>
--- a/Projects/Proj6/voltageVSccr.xlsx
+++ b/Projects/Proj6/voltageVSccr.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="13640" tabRatio="500"/>
+    <workbookView xWindow="1580" yWindow="480" windowWidth="27320" windowHeight="13640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>Rounded</t>
   </si>
@@ -41,7 +41,22 @@
     <t>Exact CCR</t>
   </si>
   <si>
-    <t>Scaled +5 *2</t>
+    <t>Scaled +5 *25.5</t>
+  </si>
+  <si>
+    <t>Scaled +5 *6.3</t>
+  </si>
+  <si>
+    <t>Round</t>
+  </si>
+  <si>
+    <t>CCR</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Scaled +5 *1.5</t>
   </si>
 </sst>
 </file>
@@ -97,8 +112,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -108,11 +127,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -309,11 +332,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-806179856"/>
-        <c:axId val="-806177536"/>
+        <c:axId val="-1651313264"/>
+        <c:axId val="-1651310944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-806179856"/>
+        <c:axId val="-1651313264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -369,12 +392,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-806177536"/>
+        <c:crossAx val="-1651310944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-806177536"/>
+        <c:axId val="-1651310944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -431,7 +454,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-806179856"/>
+        <c:crossAx val="-1651313264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -568,6 +591,20 @@
             </c:spPr>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout/>
@@ -603,7 +640,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$30:$A$40</c:f>
+              <c:f>Sheet1!$B$44:$B$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -611,41 +648,41 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51.0</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>77.0</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>102.0</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>128.0</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>153.0</c:v>
+                  <c:v>38.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>179.0</c:v>
+                  <c:v>44.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>204.0</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>230.0</c:v>
+                  <c:v>57.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>255.0</c:v>
+                  <c:v>63.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$30:$B$40</c:f>
+              <c:f>Sheet1!$D$44:$D$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -671,16 +708,16 @@
                   <c:v>11.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.399999999999998</c:v>
+                  <c:v>9.4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.599999999999999</c:v>
+                  <c:v>7.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.799999999999999</c:v>
+                  <c:v>5.8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.999999999999999</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -695,11 +732,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-805356544"/>
-        <c:axId val="-784304576"/>
+        <c:axId val="-1678108720"/>
+        <c:axId val="-1678111040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-805356544"/>
+        <c:axId val="-1678108720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -755,12 +792,412 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-784304576"/>
+        <c:crossAx val="-1678111040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-784304576"/>
+        <c:axId val="-1678111040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1678108720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$58:$A$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$58:$B$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1678066320"/>
+        <c:axId val="-1645488288"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-1678066320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1645488288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-1645488288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -816,7 +1253,406 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-805356544"/>
+        <c:crossAx val="-1678066320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$30:$A$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>102.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>153.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>179.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>204.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>230.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>255.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$30:$B$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.399999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.999999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1605807968"/>
+        <c:axId val="-1605892000"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-1605807968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1605892000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-1605892000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1605807968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -945,6 +1781,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1462,6 +2378,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2011,20 +3959,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>146050</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2034,6 +3982,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>730250</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>463550</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2305,14 +4313,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30:D40"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2617,7 +4626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <f>(A1+5)*25.5</f>
         <v>0</v>
@@ -2633,7 +4642,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" ref="A18:A27" si="6">(A2+5)*25.5</f>
         <v>25.5</v>
@@ -2650,7 +4659,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="6"/>
         <v>51</v>
@@ -2667,7 +4676,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="6"/>
         <v>76.5</v>
@@ -2684,7 +4693,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="6"/>
         <v>102</v>
@@ -2701,7 +4710,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="6"/>
         <v>127.5</v>
@@ -2717,7 +4726,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="6"/>
         <v>153</v>
@@ -2734,7 +4743,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="6"/>
         <v>178.5</v>
@@ -2751,7 +4760,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="6"/>
         <v>204</v>
@@ -2768,7 +4777,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="6"/>
         <v>229.5</v>
@@ -2785,7 +4794,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="6"/>
         <v>255</v>
@@ -2802,7 +4811,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -2810,7 +4819,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <f>ROUND(A17,0)</f>
         <v>0</v>
@@ -2827,7 +4836,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" ref="A31:A40" si="10">ROUND(A18,0)</f>
         <v>26</v>
@@ -2844,8 +4853,11 @@
         <f t="shared" ref="E31:E40" si="12">ROUND(D31,0)</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" si="10"/>
         <v>51</v>
@@ -2863,7 +4875,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" si="10"/>
         <v>77</v>
@@ -2881,7 +4893,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
         <f t="shared" si="10"/>
         <v>102</v>
@@ -2891,15 +4903,18 @@
         <v>14.599999999999996</v>
       </c>
       <c r="D34">
-        <f t="shared" si="11"/>
+        <f>-0.0667*A34+21.242</f>
         <v>14.438600000000001</v>
       </c>
       <c r="E34">
         <f t="shared" si="12"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
         <f t="shared" si="10"/>
         <v>128</v>
@@ -2916,7 +4931,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
         <f t="shared" si="10"/>
         <v>153</v>
@@ -2934,7 +4949,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37">
         <f t="shared" si="10"/>
         <v>179</v>
@@ -2952,7 +4967,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38">
         <f t="shared" si="10"/>
         <v>204</v>
@@ -2970,7 +4985,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="shared" si="10"/>
         <v>230</v>
@@ -2988,7 +5003,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40">
         <f t="shared" si="10"/>
         <v>255</v>
@@ -3003,6 +5018,452 @@
       </c>
       <c r="E40">
         <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <f>(A1+5)*6.3</f>
+        <v>0</v>
+      </c>
+      <c r="B44">
+        <f>ROUND(A44,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D44" s="1">
+        <v>21</v>
+      </c>
+      <c r="F44">
+        <f>(-0.2698*A44)+21.237</f>
+        <v>21.236999999999998</v>
+      </c>
+      <c r="G44">
+        <f>ROUND(F44,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <f t="shared" ref="A45:A54" si="15">(A2+5)*6.3</f>
+        <v>6.3</v>
+      </c>
+      <c r="B45">
+        <f t="shared" ref="B45:B54" si="16">ROUND(A45,0)</f>
+        <v>6</v>
+      </c>
+      <c r="D45" s="1">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="F45">
+        <f t="shared" ref="F45:F54" si="17">(-0.2698*A45)+21.237</f>
+        <v>19.53726</v>
+      </c>
+      <c r="G45">
+        <f t="shared" ref="G45:G54" si="18">ROUND(F45,0)</f>
+        <v>20</v>
+      </c>
+      <c r="H45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <f t="shared" si="15"/>
+        <v>12.6</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="16"/>
+        <v>13</v>
+      </c>
+      <c r="D46" s="1">
+        <v>17.8</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="17"/>
+        <v>17.837519999999998</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="18"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <f t="shared" si="15"/>
+        <v>18.899999999999999</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="16"/>
+        <v>19</v>
+      </c>
+      <c r="D47" s="1">
+        <v>16.2</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="17"/>
+        <v>16.137779999999999</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="18"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <f t="shared" si="15"/>
+        <v>25.2</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="16"/>
+        <v>25</v>
+      </c>
+      <c r="D48" s="1">
+        <v>14.6</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="17"/>
+        <v>14.438039999999999</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="18"/>
+        <v>14</v>
+      </c>
+      <c r="H48" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <f t="shared" si="15"/>
+        <v>31.5</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="16"/>
+        <v>32</v>
+      </c>
+      <c r="D49" s="1">
+        <v>13</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="17"/>
+        <v>12.738299999999999</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="18"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <f t="shared" si="15"/>
+        <v>37.799999999999997</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="16"/>
+        <v>38</v>
+      </c>
+      <c r="D50" s="1">
+        <v>11.2</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="17"/>
+        <v>11.03856</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="18"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <f t="shared" si="15"/>
+        <v>44.1</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="16"/>
+        <v>44</v>
+      </c>
+      <c r="D51" s="1">
+        <v>9.4</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="17"/>
+        <v>9.3388199999999983</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="18"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <f t="shared" si="15"/>
+        <v>50.4</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="16"/>
+        <v>50</v>
+      </c>
+      <c r="D52" s="1">
+        <v>7.6</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="17"/>
+        <v>7.6390799999999999</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="18"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <f t="shared" si="15"/>
+        <v>56.699999999999996</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="16"/>
+        <v>57</v>
+      </c>
+      <c r="D53" s="1">
+        <v>5.8</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="17"/>
+        <v>5.9393399999999996</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="18"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <f t="shared" si="15"/>
+        <v>63</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="16"/>
+        <v>63</v>
+      </c>
+      <c r="D54" s="1">
+        <v>4</v>
+      </c>
+      <c r="F54">
+        <f>(-0.2698*A54)+21.237</f>
+        <v>4.2395999999999994</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="18"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <f>(A1+5)*1.5</f>
+        <v>0</v>
+      </c>
+      <c r="B58" s="1">
+        <v>21</v>
+      </c>
+      <c r="D58">
+        <f>(-1.1333*A58)+21.227</f>
+        <v>21.227</v>
+      </c>
+      <c r="E58">
+        <f>ROUND(D58,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <f t="shared" ref="A59:A68" si="19">(A2+5)*1.5</f>
+        <v>1.5</v>
+      </c>
+      <c r="B59" s="1">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="D59">
+        <f t="shared" ref="D59:D68" si="20">(-1.1333*A59)+21.227</f>
+        <v>19.527049999999999</v>
+      </c>
+      <c r="E59">
+        <f t="shared" ref="E59:E68" si="21">ROUND(D59,0)</f>
+        <v>20</v>
+      </c>
+      <c r="F59" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <f t="shared" si="19"/>
+        <v>3</v>
+      </c>
+      <c r="B60" s="1">
+        <v>17.8</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="20"/>
+        <v>17.827100000000002</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="21"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <f t="shared" si="19"/>
+        <v>4.5</v>
+      </c>
+      <c r="B61" s="1">
+        <v>16.2</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="20"/>
+        <v>16.12715</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="21"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <f t="shared" si="19"/>
+        <v>6</v>
+      </c>
+      <c r="B62" s="1">
+        <v>14.6</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="20"/>
+        <v>14.427200000000001</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="21"/>
+        <v>14</v>
+      </c>
+      <c r="F62" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <f t="shared" si="19"/>
+        <v>7.5</v>
+      </c>
+      <c r="B63" s="1">
+        <v>13</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="20"/>
+        <v>12.72725</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="21"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <f t="shared" si="19"/>
+        <v>9</v>
+      </c>
+      <c r="B64" s="1">
+        <v>11.2</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="20"/>
+        <v>11.0273</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="21"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <f t="shared" si="19"/>
+        <v>10.5</v>
+      </c>
+      <c r="B65" s="1">
+        <v>9.4</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="20"/>
+        <v>9.3273500000000009</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <f t="shared" si="19"/>
+        <v>12</v>
+      </c>
+      <c r="B66" s="1">
+        <v>7.6</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="20"/>
+        <v>7.6274000000000015</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="21"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <f t="shared" si="19"/>
+        <v>13.5</v>
+      </c>
+      <c r="B67" s="1">
+        <v>5.8</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="20"/>
+        <v>5.9274500000000003</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="21"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <f t="shared" si="19"/>
+        <v>15</v>
+      </c>
+      <c r="B68" s="1">
+        <v>4</v>
+      </c>
+      <c r="D68">
+        <f>(-1.1333*A68)+21.227</f>
+        <v>4.2274999999999991</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="21"/>
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
LOL panel rotated pins - vin4 right down 4, agnd right down 9
</commit_message>
<xml_diff>
--- a/Projects/Proj6/voltageVSccr.xlsx
+++ b/Projects/Proj6/voltageVSccr.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zacharyweeden/Desktop/Real-Time-and-Embedded-Systems/Projects/Proj6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Real-Time-and-Embedded-Systems\Projects\Proj6\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="480" windowWidth="27320" windowHeight="13640" tabRatio="500"/>
+    <workbookView xWindow="1575" yWindow="480" windowWidth="27315" windowHeight="13635" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -144,6 +141,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -245,37 +245,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>-5.0</c:v>
+                  <c:v>-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-4.0</c:v>
+                  <c:v>-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-3.0</c:v>
+                  <c:v>-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-2.0</c:v>
+                  <c:v>-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.0</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -287,37 +287,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>21.0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.4</c:v>
+                  <c:v>19.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.8</c:v>
+                  <c:v>17.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.2</c:v>
+                  <c:v>16.199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.6</c:v>
+                  <c:v>14.599999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>11.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.399999999999998</c:v>
+                  <c:v>9.3999999999999986</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.599999999999999</c:v>
+                  <c:v>7.5999999999999988</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.799999999999999</c:v>
+                  <c:v>5.7999999999999989</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.999999999999999</c:v>
+                  <c:v>3.9999999999999991</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -332,11 +332,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1651313264"/>
-        <c:axId val="-1651310944"/>
+        <c:axId val="171232288"/>
+        <c:axId val="117664744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1651313264"/>
+        <c:axId val="171232288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -356,6 +356,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -392,12 +393,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1651310944"/>
+        <c:crossAx val="117664744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1651310944"/>
+        <c:axId val="117664744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -454,7 +455,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1651313264"/>
+        <c:crossAx val="171232288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -645,37 +646,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>38.0</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44.0</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>57.0</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>63.0</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -687,10 +688,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>21.0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.4</c:v>
+                  <c:v>19.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>17.8</c:v>
@@ -702,7 +703,7 @@
                   <c:v>14.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>11.2</c:v>
@@ -717,7 +718,7 @@
                   <c:v>5.8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -732,11 +733,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1678108720"/>
-        <c:axId val="-1678111040"/>
+        <c:axId val="172452128"/>
+        <c:axId val="172678144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1678108720"/>
+        <c:axId val="172452128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -756,6 +757,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -792,12 +794,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1678111040"/>
+        <c:crossAx val="172678144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1678111040"/>
+        <c:axId val="172678144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -854,7 +856,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1678108720"/>
+        <c:crossAx val="172452128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1045,37 +1047,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1087,10 +1089,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>21.0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.4</c:v>
+                  <c:v>19.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>17.8</c:v>
@@ -1102,7 +1104,7 @@
                   <c:v>14.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>11.2</c:v>
@@ -1117,7 +1119,7 @@
                   <c:v>5.8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1132,11 +1134,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1678066320"/>
-        <c:axId val="-1645488288"/>
+        <c:axId val="172437032"/>
+        <c:axId val="172712400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1678066320"/>
+        <c:axId val="172437032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1156,6 +1158,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1192,12 +1195,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1645488288"/>
+        <c:crossAx val="172712400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1645488288"/>
+        <c:axId val="172712400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1217,6 +1220,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1253,7 +1257,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1678066320"/>
+        <c:crossAx val="172437032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1444,37 +1448,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51.0</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>77.0</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>102.0</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>128.0</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>153.0</c:v>
+                  <c:v>153</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>179.0</c:v>
+                  <c:v>179</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>204.0</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>230.0</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>255.0</c:v>
+                  <c:v>255</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1486,37 +1490,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>21.0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.4</c:v>
+                  <c:v>19.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.8</c:v>
+                  <c:v>17.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.2</c:v>
+                  <c:v>16.199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.6</c:v>
+                  <c:v>14.599999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>11.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.399999999999998</c:v>
+                  <c:v>9.3999999999999986</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.599999999999999</c:v>
+                  <c:v>7.5999999999999988</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.799999999999999</c:v>
+                  <c:v>5.7999999999999989</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.999999999999999</c:v>
+                  <c:v>3.9999999999999991</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1531,11 +1535,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1605807968"/>
-        <c:axId val="-1605892000"/>
+        <c:axId val="172713184"/>
+        <c:axId val="172713576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1605807968"/>
+        <c:axId val="172713184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1555,6 +1559,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1591,12 +1596,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1605892000"/>
+        <c:crossAx val="172713576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1605892000"/>
+        <c:axId val="172713576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1616,6 +1621,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1652,7 +1658,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1605807968"/>
+        <c:crossAx val="172713184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3930,15 +3936,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>463550</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>82550</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>196850</xdr:rowOff>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3960,15 +3966,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:colOff>784225</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>3175</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3990,15 +3996,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>730250</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>225425</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4020,14 +4026,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>463550</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>53975</xdr:colOff>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4315,17 +4321,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="F25" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>-5</v>
       </c>
@@ -4349,7 +4355,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-4</v>
       </c>
@@ -4374,7 +4380,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-3</v>
       </c>
@@ -4399,7 +4405,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-2</v>
       </c>
@@ -4424,7 +4430,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-1</v>
       </c>
@@ -4449,7 +4455,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -4473,7 +4479,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -4498,7 +4504,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -4523,7 +4529,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -4548,7 +4554,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -4573,7 +4579,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -4598,7 +4604,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>1</v>
       </c>
@@ -4612,7 +4618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -4626,7 +4632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>(A1+5)*25.5</f>
         <v>0</v>
@@ -4642,7 +4648,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ref="A18:A27" si="6">(A2+5)*25.5</f>
         <v>25.5</v>
@@ -4659,7 +4665,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="6"/>
         <v>51</v>
@@ -4676,7 +4682,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="6"/>
         <v>76.5</v>
@@ -4693,7 +4699,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="6"/>
         <v>102</v>
@@ -4710,7 +4716,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="6"/>
         <v>127.5</v>
@@ -4726,7 +4732,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="6"/>
         <v>153</v>
@@ -4743,7 +4749,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="6"/>
         <v>178.5</v>
@@ -4760,7 +4766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="6"/>
         <v>204</v>
@@ -4777,7 +4783,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="6"/>
         <v>229.5</v>
@@ -4794,7 +4800,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="6"/>
         <v>255</v>
@@ -4811,7 +4817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -4819,7 +4825,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <f>ROUND(A17,0)</f>
         <v>0</v>
@@ -4836,7 +4842,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" ref="A31:A40" si="10">ROUND(A18,0)</f>
         <v>26</v>
@@ -4857,7 +4863,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="10"/>
         <v>51</v>
@@ -4875,7 +4881,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="10"/>
         <v>77</v>
@@ -4893,7 +4899,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="10"/>
         <v>102</v>
@@ -4914,7 +4920,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="10"/>
         <v>128</v>
@@ -4931,7 +4937,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="10"/>
         <v>153</v>
@@ -4949,7 +4955,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="10"/>
         <v>179</v>
@@ -4967,7 +4973,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="10"/>
         <v>204</v>
@@ -4985,7 +4991,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="10"/>
         <v>230</v>
@@ -5003,7 +5009,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="10"/>
         <v>255</v>
@@ -5021,7 +5027,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>5</v>
       </c>
@@ -5032,7 +5038,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <f>(A1+5)*6.3</f>
         <v>0</v>
@@ -5053,7 +5059,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" ref="A45:A54" si="15">(A2+5)*6.3</f>
         <v>6.3</v>
@@ -5066,7 +5072,7 @@
         <v>19.399999999999999</v>
       </c>
       <c r="F45">
-        <f t="shared" ref="F45:F54" si="17">(-0.2698*A45)+21.237</f>
+        <f t="shared" ref="F45:F53" si="17">(-0.2698*A45)+21.237</f>
         <v>19.53726</v>
       </c>
       <c r="G45">
@@ -5077,7 +5083,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="15"/>
         <v>12.6</v>
@@ -5098,7 +5104,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="15"/>
         <v>18.899999999999999</v>
@@ -5119,7 +5125,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="15"/>
         <v>25.2</v>
@@ -5143,7 +5149,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="15"/>
         <v>31.5</v>
@@ -5164,7 +5170,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="15"/>
         <v>37.799999999999997</v>
@@ -5185,7 +5191,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="15"/>
         <v>44.1</v>
@@ -5206,7 +5212,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="15"/>
         <v>50.4</v>
@@ -5227,7 +5233,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="15"/>
         <v>56.699999999999996</v>
@@ -5248,7 +5254,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="15"/>
         <v>63</v>
@@ -5269,12 +5275,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <f>(A1+5)*1.5</f>
         <v>0</v>
@@ -5291,7 +5297,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" ref="A59:A68" si="19">(A2+5)*1.5</f>
         <v>1.5</v>
@@ -5300,7 +5306,7 @@
         <v>19.399999999999999</v>
       </c>
       <c r="D59">
-        <f t="shared" ref="D59:D68" si="20">(-1.1333*A59)+21.227</f>
+        <f t="shared" ref="D59:D67" si="20">(-1.1333*A59)+21.227</f>
         <v>19.527049999999999</v>
       </c>
       <c r="E59">
@@ -5311,7 +5317,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="19"/>
         <v>3</v>
@@ -5328,7 +5334,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" si="19"/>
         <v>4.5</v>
@@ -5345,7 +5351,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="19"/>
         <v>6</v>
@@ -5365,7 +5371,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" si="19"/>
         <v>7.5</v>
@@ -5382,7 +5388,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="19"/>
         <v>9</v>
@@ -5399,7 +5405,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" si="19"/>
         <v>10.5</v>
@@ -5416,7 +5422,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="19"/>
         <v>12</v>
@@ -5433,7 +5439,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" si="19"/>
         <v>13.5</v>
@@ -5450,7 +5456,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" si="19"/>
         <v>15</v>

</xml_diff>